<commit_message>
Add template slide & update tasklist
Slide: Sơn + Mạnh
WBS: Khôi
</commit_message>
<xml_diff>
--- a/Document/TasklistAss1.xlsx
+++ b/Document/TasklistAss1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
   <si>
     <t>Tasks</t>
   </si>
@@ -809,7 +809,7 @@
   <dimension ref="A1:BB98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1027,7 +1027,7 @@
         <v>42780</v>
       </c>
       <c r="F5" s="7">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>7</v>
@@ -1084,7 +1084,7 @@
         <v>42780</v>
       </c>
       <c r="F6" s="7">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>7</v>
@@ -1141,10 +1141,10 @@
         <v>42781</v>
       </c>
       <c r="F7" s="7">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1198,10 +1198,10 @@
         <v>42781</v>
       </c>
       <c r="F8" s="7">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1314,7 +1314,9 @@
       <c r="F10" s="7">
         <v>0</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>

</xml_diff>